<commit_message>
Project SprBeanTest2 is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/SprBeanTest2/SprBeanTest.xlsx
+++ b/DESIGN/rules/SprBeanTest2/SprBeanTest.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Result</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>Spreadsheet AnySpreadsheetResult mainSpr2(SpreadsheetResult a)</t>
+  </si>
+  <si>
+    <t>Spreadsheet AnySpreadsheetResult mainSpr2()</t>
+  </si>
+  <si>
+    <t>=someSpr2()</t>
+  </si>
+  <si>
+    <t>=someSpr2(100)</t>
   </si>
 </sst>
 </file>
@@ -549,7 +558,7 @@
     <row r="11" spans="4:11" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F23" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G23" s="4"/>
     </row>
@@ -566,7 +575,7 @@
         <v>4</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>